<commit_message>
covid-19 update march 11
</commit_message>
<xml_diff>
--- a/COVID-19_DATA.xlsx
+++ b/COVID-19_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2648" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="16">
   <si>
     <t>Cumulative  Test positive</t>
   </si>
@@ -1000,13 +1000,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I2640"/>
+  <dimension ref="A1:I2654"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2624" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2636" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2642" sqref="C2642"/>
+      <selection pane="bottomRight" activeCell="K2651" sqref="K2651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88117,6 +88117,468 @@
         <v>2206</v>
       </c>
     </row>
+    <row r="2641" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2641" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2641" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2641">
+        <v>10673</v>
+      </c>
+      <c r="D2641">
+        <v>314</v>
+      </c>
+      <c r="E2641">
+        <v>9628</v>
+      </c>
+      <c r="F2641" s="26">
+        <f t="shared" ref="F2641:F2654" si="219">C2641-D2641-E2641</f>
+        <v>731</v>
+      </c>
+      <c r="G2641" s="19">
+        <f t="shared" ref="G2641:G2654" si="220">C2641-C2634</f>
+        <v>47</v>
+      </c>
+      <c r="H2641" s="15">
+        <f t="shared" ref="H2641:H2654" si="221">D2641-D2634</f>
+        <v>1</v>
+      </c>
+      <c r="I2641" s="23">
+        <f t="shared" ref="I2641:I2654" si="222">E2641-E2634</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2642" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2642" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2642">
+        <v>19141</v>
+      </c>
+      <c r="D2642">
+        <v>202</v>
+      </c>
+      <c r="E2642">
+        <v>18842</v>
+      </c>
+      <c r="F2642" s="26">
+        <f t="shared" si="219"/>
+        <v>97</v>
+      </c>
+      <c r="G2642" s="19">
+        <f t="shared" si="220"/>
+        <v>20</v>
+      </c>
+      <c r="H2642" s="15">
+        <f t="shared" si="221"/>
+        <v>1</v>
+      </c>
+      <c r="I2642" s="23">
+        <f t="shared" si="222"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2643" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2643" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2643">
+        <v>4959</v>
+      </c>
+      <c r="D2643">
+        <v>103</v>
+      </c>
+      <c r="E2643">
+        <v>4853</v>
+      </c>
+      <c r="F2643" s="26">
+        <f t="shared" si="219"/>
+        <v>3</v>
+      </c>
+      <c r="G2643" s="19">
+        <f t="shared" si="220"/>
+        <v>0</v>
+      </c>
+      <c r="H2643" s="15">
+        <f t="shared" si="221"/>
+        <v>1</v>
+      </c>
+      <c r="I2643" s="23">
+        <f t="shared" si="222"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2644" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2644" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2644">
+        <v>46229</v>
+      </c>
+      <c r="D2644">
+        <v>512</v>
+      </c>
+      <c r="E2644">
+        <v>43244</v>
+      </c>
+      <c r="F2644" s="26">
+        <f t="shared" si="219"/>
+        <v>2473</v>
+      </c>
+      <c r="G2644" s="19">
+        <f t="shared" si="220"/>
+        <v>253</v>
+      </c>
+      <c r="H2644" s="15">
+        <f t="shared" si="221"/>
+        <v>1</v>
+      </c>
+      <c r="I2644" s="23">
+        <f t="shared" si="222"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2645" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2645" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2645">
+        <v>74433</v>
+      </c>
+      <c r="D2645">
+        <v>2122</v>
+      </c>
+      <c r="E2645">
+        <v>69849</v>
+      </c>
+      <c r="F2645" s="26">
+        <f t="shared" si="219"/>
+        <v>2462</v>
+      </c>
+      <c r="G2645" s="19">
+        <f t="shared" si="220"/>
+        <v>266</v>
+      </c>
+      <c r="H2645" s="15">
+        <f t="shared" si="221"/>
+        <v>4</v>
+      </c>
+      <c r="I2645" s="23">
+        <f t="shared" si="222"/>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2646" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2646" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2646">
+        <v>179654</v>
+      </c>
+      <c r="D2646">
+        <v>5629</v>
+      </c>
+      <c r="E2646">
+        <v>167269</v>
+      </c>
+      <c r="F2646" s="26">
+        <f t="shared" si="219"/>
+        <v>6756</v>
+      </c>
+      <c r="G2646" s="19">
+        <f t="shared" si="220"/>
+        <v>1006</v>
+      </c>
+      <c r="H2646" s="15">
+        <f t="shared" si="221"/>
+        <v>29</v>
+      </c>
+      <c r="I2646" s="23">
+        <f t="shared" si="222"/>
+        <v>766</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2647" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2647" s="8">
+        <v>44264</v>
+      </c>
+      <c r="C2647">
+        <v>260150</v>
+      </c>
+      <c r="D2647">
+        <v>4442</v>
+      </c>
+      <c r="E2647">
+        <v>251531</v>
+      </c>
+      <c r="F2647" s="26">
+        <f t="shared" si="219"/>
+        <v>4177</v>
+      </c>
+      <c r="G2647" s="19">
+        <f t="shared" si="220"/>
+        <v>194</v>
+      </c>
+      <c r="H2647" s="15">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
+      <c r="I2647" s="23">
+        <f t="shared" si="222"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2648" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2648" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2648">
+        <v>10730</v>
+      </c>
+      <c r="D2648">
+        <v>316</v>
+      </c>
+      <c r="E2648">
+        <v>9673</v>
+      </c>
+      <c r="F2648" s="26">
+        <f t="shared" si="219"/>
+        <v>741</v>
+      </c>
+      <c r="G2648" s="19">
+        <f t="shared" si="220"/>
+        <v>57</v>
+      </c>
+      <c r="H2648" s="15">
+        <f t="shared" si="221"/>
+        <v>2</v>
+      </c>
+      <c r="I2648" s="23">
+        <f t="shared" si="222"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2649" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2649" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2649">
+        <v>19157</v>
+      </c>
+      <c r="D2649">
+        <v>202</v>
+      </c>
+      <c r="E2649">
+        <v>18845</v>
+      </c>
+      <c r="F2649" s="26">
+        <f t="shared" si="219"/>
+        <v>110</v>
+      </c>
+      <c r="G2649" s="19">
+        <f t="shared" si="220"/>
+        <v>16</v>
+      </c>
+      <c r="H2649" s="15">
+        <f t="shared" si="221"/>
+        <v>0</v>
+      </c>
+      <c r="I2649" s="23">
+        <f t="shared" si="222"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2650" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2650" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2650">
+        <v>4959</v>
+      </c>
+      <c r="D2650">
+        <v>104</v>
+      </c>
+      <c r="E2650">
+        <v>4855</v>
+      </c>
+      <c r="F2650" s="26">
+        <f t="shared" si="219"/>
+        <v>0</v>
+      </c>
+      <c r="G2650" s="19">
+        <f t="shared" si="220"/>
+        <v>0</v>
+      </c>
+      <c r="H2650" s="15">
+        <f t="shared" si="221"/>
+        <v>1</v>
+      </c>
+      <c r="I2650" s="23">
+        <f t="shared" si="222"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2651" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2651" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2651">
+        <v>46579</v>
+      </c>
+      <c r="D2651">
+        <v>516</v>
+      </c>
+      <c r="E2651">
+        <v>43435</v>
+      </c>
+      <c r="F2651" s="26">
+        <f t="shared" si="219"/>
+        <v>2628</v>
+      </c>
+      <c r="G2651" s="19">
+        <f t="shared" si="220"/>
+        <v>350</v>
+      </c>
+      <c r="H2651" s="15">
+        <f t="shared" si="221"/>
+        <v>4</v>
+      </c>
+      <c r="I2651" s="23">
+        <f t="shared" si="222"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2652" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2652" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2652">
+        <v>74722</v>
+      </c>
+      <c r="D2652">
+        <v>2129</v>
+      </c>
+      <c r="E2652">
+        <v>70044</v>
+      </c>
+      <c r="F2652" s="26">
+        <f t="shared" si="219"/>
+        <v>2549</v>
+      </c>
+      <c r="G2652" s="19">
+        <f t="shared" si="220"/>
+        <v>289</v>
+      </c>
+      <c r="H2652" s="15">
+        <f t="shared" si="221"/>
+        <v>7</v>
+      </c>
+      <c r="I2652" s="23">
+        <f t="shared" si="222"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2653" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2653" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2653">
+        <v>180944</v>
+      </c>
+      <c r="D2653">
+        <v>5662</v>
+      </c>
+      <c r="E2653">
+        <v>167967</v>
+      </c>
+      <c r="F2653" s="26">
+        <f t="shared" si="219"/>
+        <v>7315</v>
+      </c>
+      <c r="G2653" s="19">
+        <f t="shared" si="220"/>
+        <v>1290</v>
+      </c>
+      <c r="H2653" s="15">
+        <f t="shared" si="221"/>
+        <v>33</v>
+      </c>
+      <c r="I2653" s="23">
+        <f t="shared" si="222"/>
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2654" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2654" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C2654">
+        <v>260406</v>
+      </c>
+      <c r="D2654">
+        <v>4448</v>
+      </c>
+      <c r="E2654">
+        <v>251673</v>
+      </c>
+      <c r="F2654" s="26">
+        <f t="shared" si="219"/>
+        <v>4285</v>
+      </c>
+      <c r="G2654" s="19">
+        <f t="shared" si="220"/>
+        <v>256</v>
+      </c>
+      <c r="H2654" s="15">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
+      <c r="I2654" s="23">
+        <f t="shared" si="222"/>
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:H3313">
     <sortCondition ref="B2:B3313"/>

</xml_diff>

<commit_message>
march 16, 2021 - update
</commit_message>
<xml_diff>
--- a/COVID-19_DATA.xlsx
+++ b/COVID-19_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="16">
   <si>
     <t>Cumulative  Test positive</t>
   </si>
@@ -1000,13 +1000,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I2654"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2636" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2678" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2651" sqref="K2651"/>
+      <selection pane="bottomRight" activeCell="C2690" sqref="C2690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88134,7 +88134,7 @@
         <v>9628</v>
       </c>
       <c r="F2641" s="26">
-        <f t="shared" ref="F2641:F2654" si="219">C2641-D2641-E2641</f>
+        <f t="shared" ref="F2641:F2661" si="219">C2641-D2641-E2641</f>
         <v>731</v>
       </c>
       <c r="G2641" s="19">
@@ -88425,14 +88425,14 @@
         <v>4959</v>
       </c>
       <c r="D2650">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E2650">
         <v>4855</v>
       </c>
       <c r="F2650" s="26">
         <f t="shared" si="219"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2650" s="19">
         <f t="shared" si="220"/>
@@ -88440,7 +88440,7 @@
       </c>
       <c r="H2650" s="15">
         <f t="shared" si="221"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2650" s="23">
         <f t="shared" si="222"/>
@@ -88577,6 +88577,1222 @@
       <c r="I2654" s="23">
         <f t="shared" si="222"/>
         <v>142</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2655" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2655" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2655">
+        <v>10816</v>
+      </c>
+      <c r="D2655">
+        <v>317</v>
+      </c>
+      <c r="E2655">
+        <v>9739</v>
+      </c>
+      <c r="F2655" s="26">
+        <f t="shared" si="219"/>
+        <v>760</v>
+      </c>
+      <c r="G2655" s="19">
+        <f t="shared" ref="G2655:G2661" si="223">C2655-C2648</f>
+        <v>86</v>
+      </c>
+      <c r="H2655" s="15">
+        <f t="shared" ref="H2655:H2661" si="224">D2655-D2648</f>
+        <v>1</v>
+      </c>
+      <c r="I2655" s="23">
+        <f t="shared" ref="I2655:I2661" si="225">E2655-E2648</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2656" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2656" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2656">
+        <v>19171</v>
+      </c>
+      <c r="D2656">
+        <v>202</v>
+      </c>
+      <c r="E2656">
+        <v>18849</v>
+      </c>
+      <c r="F2656" s="26">
+        <f t="shared" si="219"/>
+        <v>120</v>
+      </c>
+      <c r="G2656" s="19">
+        <f t="shared" si="223"/>
+        <v>14</v>
+      </c>
+      <c r="H2656" s="15">
+        <f t="shared" si="224"/>
+        <v>0</v>
+      </c>
+      <c r="I2656" s="23">
+        <f t="shared" si="225"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2657" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2657" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2657">
+        <v>4959</v>
+      </c>
+      <c r="D2657">
+        <v>103</v>
+      </c>
+      <c r="E2657">
+        <v>4856</v>
+      </c>
+      <c r="F2657" s="26">
+        <f t="shared" si="219"/>
+        <v>0</v>
+      </c>
+      <c r="G2657" s="19">
+        <f t="shared" si="223"/>
+        <v>0</v>
+      </c>
+      <c r="H2657" s="15">
+        <f t="shared" si="224"/>
+        <v>0</v>
+      </c>
+      <c r="I2657" s="23">
+        <f t="shared" si="225"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2658" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2658" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2658">
+        <v>46963</v>
+      </c>
+      <c r="D2658">
+        <v>520</v>
+      </c>
+      <c r="E2658">
+        <v>43658</v>
+      </c>
+      <c r="F2658" s="26">
+        <f t="shared" si="219"/>
+        <v>2785</v>
+      </c>
+      <c r="G2658" s="19">
+        <f t="shared" si="223"/>
+        <v>384</v>
+      </c>
+      <c r="H2658" s="15">
+        <f t="shared" si="224"/>
+        <v>4</v>
+      </c>
+      <c r="I2658" s="23">
+        <f t="shared" si="225"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2659" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2659" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2659">
+        <v>75052</v>
+      </c>
+      <c r="D2659">
+        <v>2138</v>
+      </c>
+      <c r="E2659">
+        <v>70245</v>
+      </c>
+      <c r="F2659" s="26">
+        <f t="shared" si="219"/>
+        <v>2669</v>
+      </c>
+      <c r="G2659" s="19">
+        <f t="shared" si="223"/>
+        <v>330</v>
+      </c>
+      <c r="H2659" s="15">
+        <f t="shared" si="224"/>
+        <v>9</v>
+      </c>
+      <c r="I2659" s="23">
+        <f t="shared" si="225"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2660" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2660" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2660">
+        <v>182576</v>
+      </c>
+      <c r="D2660">
+        <v>5698</v>
+      </c>
+      <c r="E2660">
+        <v>168186</v>
+      </c>
+      <c r="F2660" s="26">
+        <f t="shared" si="219"/>
+        <v>8692</v>
+      </c>
+      <c r="G2660" s="19">
+        <f t="shared" si="223"/>
+        <v>1632</v>
+      </c>
+      <c r="H2660" s="15">
+        <f t="shared" si="224"/>
+        <v>36</v>
+      </c>
+      <c r="I2660" s="23">
+        <f t="shared" si="225"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2661" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2661" s="8">
+        <v>44266</v>
+      </c>
+      <c r="C2661">
+        <v>260661</v>
+      </c>
+      <c r="D2661">
+        <v>4452</v>
+      </c>
+      <c r="E2661">
+        <v>252532</v>
+      </c>
+      <c r="F2661" s="26">
+        <f t="shared" si="219"/>
+        <v>3677</v>
+      </c>
+      <c r="G2661" s="19">
+        <f t="shared" si="223"/>
+        <v>255</v>
+      </c>
+      <c r="H2661" s="15">
+        <f t="shared" si="224"/>
+        <v>4</v>
+      </c>
+      <c r="I2661" s="23">
+        <f t="shared" si="225"/>
+        <v>859</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2662" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2662" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2662">
+        <v>10892</v>
+      </c>
+      <c r="D2662">
+        <v>317</v>
+      </c>
+      <c r="E2662">
+        <v>9808</v>
+      </c>
+      <c r="F2662" s="26">
+        <f t="shared" ref="F2662:F2689" si="226">C2662-D2662-E2662</f>
+        <v>767</v>
+      </c>
+      <c r="G2662" s="19">
+        <f t="shared" ref="G2662:G2682" si="227">C2662-C2655</f>
+        <v>76</v>
+      </c>
+      <c r="H2662" s="15">
+        <f t="shared" ref="H2662:H2682" si="228">D2662-D2655</f>
+        <v>0</v>
+      </c>
+      <c r="I2662" s="23">
+        <f t="shared" ref="I2662:I2682" si="229">E2662-E2655</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2663" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2663" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2663">
+        <v>19188</v>
+      </c>
+      <c r="D2663">
+        <v>202</v>
+      </c>
+      <c r="E2663">
+        <v>18860</v>
+      </c>
+      <c r="F2663" s="26">
+        <f t="shared" si="226"/>
+        <v>126</v>
+      </c>
+      <c r="G2663" s="19">
+        <f t="shared" si="227"/>
+        <v>17</v>
+      </c>
+      <c r="H2663" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2663" s="23">
+        <f t="shared" si="229"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2664" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2664" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2664">
+        <v>4960</v>
+      </c>
+      <c r="D2664">
+        <v>103</v>
+      </c>
+      <c r="E2664">
+        <v>4856</v>
+      </c>
+      <c r="F2664" s="26">
+        <f t="shared" si="226"/>
+        <v>1</v>
+      </c>
+      <c r="G2664" s="19">
+        <f t="shared" si="227"/>
+        <v>1</v>
+      </c>
+      <c r="H2664" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2664" s="23">
+        <f t="shared" si="229"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2665" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2665" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2665">
+        <v>47365</v>
+      </c>
+      <c r="D2665">
+        <v>522</v>
+      </c>
+      <c r="E2665">
+        <v>43808</v>
+      </c>
+      <c r="F2665" s="26">
+        <f t="shared" si="226"/>
+        <v>3035</v>
+      </c>
+      <c r="G2665" s="19">
+        <f t="shared" si="227"/>
+        <v>402</v>
+      </c>
+      <c r="H2665" s="15">
+        <f t="shared" si="228"/>
+        <v>2</v>
+      </c>
+      <c r="I2665" s="23">
+        <f t="shared" si="229"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2666" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2666" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2666">
+        <v>75357</v>
+      </c>
+      <c r="D2666">
+        <v>2147</v>
+      </c>
+      <c r="E2666">
+        <v>70360</v>
+      </c>
+      <c r="F2666" s="26">
+        <f t="shared" si="226"/>
+        <v>2850</v>
+      </c>
+      <c r="G2666" s="19">
+        <f t="shared" si="227"/>
+        <v>305</v>
+      </c>
+      <c r="H2666" s="15">
+        <f t="shared" si="228"/>
+        <v>9</v>
+      </c>
+      <c r="I2666" s="23">
+        <f t="shared" si="229"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2667" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2667" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2667">
+        <v>183815</v>
+      </c>
+      <c r="D2667">
+        <v>5732</v>
+      </c>
+      <c r="E2667">
+        <v>168979</v>
+      </c>
+      <c r="F2667" s="26">
+        <f t="shared" si="226"/>
+        <v>9104</v>
+      </c>
+      <c r="G2667" s="19">
+        <f t="shared" si="227"/>
+        <v>1239</v>
+      </c>
+      <c r="H2667" s="15">
+        <f t="shared" si="228"/>
+        <v>34</v>
+      </c>
+      <c r="I2667" s="23">
+        <f t="shared" si="229"/>
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2668" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2668" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C2668">
+        <v>260959</v>
+      </c>
+      <c r="D2668">
+        <v>4453</v>
+      </c>
+      <c r="E2668">
+        <v>252625</v>
+      </c>
+      <c r="F2668" s="26">
+        <f t="shared" si="226"/>
+        <v>3881</v>
+      </c>
+      <c r="G2668" s="19">
+        <f t="shared" si="227"/>
+        <v>298</v>
+      </c>
+      <c r="H2668" s="15">
+        <f t="shared" si="228"/>
+        <v>1</v>
+      </c>
+      <c r="I2668" s="23">
+        <f t="shared" si="229"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2669" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2669" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2669">
+        <v>10952</v>
+      </c>
+      <c r="D2669">
+        <v>320</v>
+      </c>
+      <c r="E2669">
+        <v>9864</v>
+      </c>
+      <c r="F2669" s="26">
+        <f t="shared" si="226"/>
+        <v>768</v>
+      </c>
+      <c r="G2669" s="19">
+        <f t="shared" si="227"/>
+        <v>60</v>
+      </c>
+      <c r="H2669" s="15">
+        <f t="shared" si="228"/>
+        <v>3</v>
+      </c>
+      <c r="I2669" s="23">
+        <f t="shared" si="229"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2670" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2670" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2670">
+        <v>19206</v>
+      </c>
+      <c r="D2670">
+        <v>202</v>
+      </c>
+      <c r="E2670">
+        <v>18868</v>
+      </c>
+      <c r="F2670" s="26">
+        <f t="shared" si="226"/>
+        <v>136</v>
+      </c>
+      <c r="G2670" s="19">
+        <f t="shared" si="227"/>
+        <v>18</v>
+      </c>
+      <c r="H2670" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2670" s="23">
+        <f t="shared" si="229"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2671" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2671" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2671">
+        <v>4960</v>
+      </c>
+      <c r="D2671">
+        <v>103</v>
+      </c>
+      <c r="E2671">
+        <v>4856</v>
+      </c>
+      <c r="F2671" s="26">
+        <f t="shared" si="226"/>
+        <v>1</v>
+      </c>
+      <c r="G2671" s="19">
+        <f t="shared" si="227"/>
+        <v>0</v>
+      </c>
+      <c r="H2671" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2671" s="23">
+        <f t="shared" si="229"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2672" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2672" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2672">
+        <v>47710</v>
+      </c>
+      <c r="D2672">
+        <v>524</v>
+      </c>
+      <c r="E2672">
+        <v>44043</v>
+      </c>
+      <c r="F2672" s="26">
+        <f t="shared" si="226"/>
+        <v>3143</v>
+      </c>
+      <c r="G2672" s="19">
+        <f t="shared" si="227"/>
+        <v>345</v>
+      </c>
+      <c r="H2672" s="15">
+        <f t="shared" si="228"/>
+        <v>2</v>
+      </c>
+      <c r="I2672" s="23">
+        <f t="shared" si="229"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2673" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2673" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2673">
+        <v>75725</v>
+      </c>
+      <c r="D2673">
+        <v>2153</v>
+      </c>
+      <c r="E2673">
+        <v>70514</v>
+      </c>
+      <c r="F2673" s="26">
+        <f t="shared" si="226"/>
+        <v>3058</v>
+      </c>
+      <c r="G2673" s="19">
+        <f t="shared" si="227"/>
+        <v>368</v>
+      </c>
+      <c r="H2673" s="15">
+        <f t="shared" si="228"/>
+        <v>6</v>
+      </c>
+      <c r="I2673" s="23">
+        <f t="shared" si="229"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2674" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2674" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2674">
+        <v>185468</v>
+      </c>
+      <c r="D2674">
+        <v>5753</v>
+      </c>
+      <c r="E2674">
+        <v>169752</v>
+      </c>
+      <c r="F2674" s="26">
+        <f t="shared" si="226"/>
+        <v>9963</v>
+      </c>
+      <c r="G2674" s="19">
+        <f t="shared" si="227"/>
+        <v>1653</v>
+      </c>
+      <c r="H2674" s="15">
+        <f t="shared" si="228"/>
+        <v>21</v>
+      </c>
+      <c r="I2674" s="23">
+        <f t="shared" si="229"/>
+        <v>773</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2675" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2675" s="8">
+        <v>44268</v>
+      </c>
+      <c r="C2675">
+        <v>261179</v>
+      </c>
+      <c r="D2675">
+        <v>4453</v>
+      </c>
+      <c r="E2675">
+        <v>252674</v>
+      </c>
+      <c r="F2675" s="26">
+        <f t="shared" si="226"/>
+        <v>4052</v>
+      </c>
+      <c r="G2675" s="19">
+        <f t="shared" si="227"/>
+        <v>220</v>
+      </c>
+      <c r="H2675" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2675" s="23">
+        <f t="shared" si="229"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2676" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2676" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2676">
+        <v>11017</v>
+      </c>
+      <c r="D2676">
+        <v>320</v>
+      </c>
+      <c r="E2676">
+        <v>9926</v>
+      </c>
+      <c r="F2676" s="26">
+        <f t="shared" si="226"/>
+        <v>771</v>
+      </c>
+      <c r="G2676" s="19">
+        <f t="shared" si="227"/>
+        <v>65</v>
+      </c>
+      <c r="H2676" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2676" s="23">
+        <f t="shared" si="229"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2677" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2677" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2677">
+        <v>19220</v>
+      </c>
+      <c r="D2677">
+        <v>202</v>
+      </c>
+      <c r="E2677">
+        <v>18881</v>
+      </c>
+      <c r="F2677" s="26">
+        <f t="shared" si="226"/>
+        <v>137</v>
+      </c>
+      <c r="G2677" s="19">
+        <f t="shared" si="227"/>
+        <v>14</v>
+      </c>
+      <c r="H2677" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2677" s="23">
+        <f t="shared" si="229"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2678" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2678" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2678">
+        <v>4961</v>
+      </c>
+      <c r="D2678">
+        <v>103</v>
+      </c>
+      <c r="E2678">
+        <v>4856</v>
+      </c>
+      <c r="F2678" s="26">
+        <f t="shared" si="226"/>
+        <v>2</v>
+      </c>
+      <c r="G2678" s="19">
+        <f t="shared" si="227"/>
+        <v>1</v>
+      </c>
+      <c r="H2678" s="15">
+        <f t="shared" si="228"/>
+        <v>0</v>
+      </c>
+      <c r="I2678" s="23">
+        <f t="shared" si="229"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2679" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2679" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2679">
+        <v>48081</v>
+      </c>
+      <c r="D2679">
+        <v>526</v>
+      </c>
+      <c r="E2679">
+        <v>44152</v>
+      </c>
+      <c r="F2679" s="26">
+        <f t="shared" si="226"/>
+        <v>3403</v>
+      </c>
+      <c r="G2679" s="19">
+        <f t="shared" si="227"/>
+        <v>371</v>
+      </c>
+      <c r="H2679" s="15">
+        <f t="shared" si="228"/>
+        <v>2</v>
+      </c>
+      <c r="I2679" s="23">
+        <f t="shared" si="229"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2680" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2680" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2680">
+        <v>76104</v>
+      </c>
+      <c r="D2680">
+        <v>2159</v>
+      </c>
+      <c r="E2680">
+        <v>70655</v>
+      </c>
+      <c r="F2680" s="26">
+        <f t="shared" si="226"/>
+        <v>3290</v>
+      </c>
+      <c r="G2680" s="19">
+        <f t="shared" si="227"/>
+        <v>379</v>
+      </c>
+      <c r="H2680" s="15">
+        <f t="shared" si="228"/>
+        <v>6</v>
+      </c>
+      <c r="I2680" s="23">
+        <f t="shared" si="229"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2681" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2681" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2681">
+        <v>186659</v>
+      </c>
+      <c r="D2681">
+        <v>5769</v>
+      </c>
+      <c r="E2681">
+        <v>170695</v>
+      </c>
+      <c r="F2681" s="26">
+        <f t="shared" si="226"/>
+        <v>10195</v>
+      </c>
+      <c r="G2681" s="19">
+        <f t="shared" si="227"/>
+        <v>1191</v>
+      </c>
+      <c r="H2681" s="15">
+        <f t="shared" si="228"/>
+        <v>16</v>
+      </c>
+      <c r="I2681" s="23">
+        <f t="shared" si="229"/>
+        <v>943</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2682" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2682" s="8">
+        <v>44269</v>
+      </c>
+      <c r="C2682">
+        <v>261411</v>
+      </c>
+      <c r="D2682">
+        <v>4458</v>
+      </c>
+      <c r="E2682">
+        <v>252713</v>
+      </c>
+      <c r="F2682" s="26">
+        <f t="shared" si="226"/>
+        <v>4240</v>
+      </c>
+      <c r="G2682" s="19">
+        <f t="shared" si="227"/>
+        <v>232</v>
+      </c>
+      <c r="H2682" s="15">
+        <f t="shared" si="228"/>
+        <v>5</v>
+      </c>
+      <c r="I2682" s="23">
+        <f t="shared" si="229"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2683" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2683" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2683">
+        <v>11089</v>
+      </c>
+      <c r="D2683">
+        <v>322</v>
+      </c>
+      <c r="E2683">
+        <v>9985</v>
+      </c>
+      <c r="F2683" s="26">
+        <f t="shared" si="226"/>
+        <v>782</v>
+      </c>
+      <c r="G2683" s="19">
+        <f t="shared" ref="G2683:G2689" si="230">C2683-C2676</f>
+        <v>72</v>
+      </c>
+      <c r="H2683" s="15">
+        <f t="shared" ref="H2683:H2689" si="231">D2683-D2676</f>
+        <v>2</v>
+      </c>
+      <c r="I2683" s="23">
+        <f t="shared" ref="I2683:I2689" si="232">E2683-E2676</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2684" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2684" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2684">
+        <v>19233</v>
+      </c>
+      <c r="D2684">
+        <v>202</v>
+      </c>
+      <c r="E2684">
+        <v>18890</v>
+      </c>
+      <c r="F2684" s="26">
+        <f t="shared" si="226"/>
+        <v>141</v>
+      </c>
+      <c r="G2684" s="19">
+        <f t="shared" si="230"/>
+        <v>13</v>
+      </c>
+      <c r="H2684" s="15">
+        <f t="shared" si="231"/>
+        <v>0</v>
+      </c>
+      <c r="I2684" s="23">
+        <f t="shared" si="232"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2685" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2685" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2685">
+        <v>4961</v>
+      </c>
+      <c r="D2685">
+        <v>103</v>
+      </c>
+      <c r="E2685">
+        <v>4856</v>
+      </c>
+      <c r="F2685" s="26">
+        <f t="shared" si="226"/>
+        <v>2</v>
+      </c>
+      <c r="G2685" s="19">
+        <f t="shared" si="230"/>
+        <v>0</v>
+      </c>
+      <c r="H2685" s="15">
+        <f t="shared" si="231"/>
+        <v>0</v>
+      </c>
+      <c r="I2685" s="23">
+        <f t="shared" si="232"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2686" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2686" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2686">
+        <v>48495</v>
+      </c>
+      <c r="D2686">
+        <v>526</v>
+      </c>
+      <c r="E2686">
+        <v>44409</v>
+      </c>
+      <c r="F2686" s="26">
+        <f t="shared" si="226"/>
+        <v>3560</v>
+      </c>
+      <c r="G2686" s="19">
+        <f t="shared" si="230"/>
+        <v>414</v>
+      </c>
+      <c r="H2686" s="15">
+        <f t="shared" si="231"/>
+        <v>0</v>
+      </c>
+      <c r="I2686" s="23">
+        <f t="shared" si="232"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2687" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2687" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2687">
+        <v>76379</v>
+      </c>
+      <c r="D2687">
+        <v>2169</v>
+      </c>
+      <c r="E2687">
+        <v>70861</v>
+      </c>
+      <c r="F2687" s="26">
+        <f t="shared" si="226"/>
+        <v>3349</v>
+      </c>
+      <c r="G2687" s="19">
+        <f t="shared" si="230"/>
+        <v>275</v>
+      </c>
+      <c r="H2687" s="15">
+        <f t="shared" si="231"/>
+        <v>10</v>
+      </c>
+      <c r="I2687" s="23">
+        <f t="shared" si="232"/>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2688" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2688" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2688">
+        <v>188225</v>
+      </c>
+      <c r="D2688">
+        <v>5812</v>
+      </c>
+      <c r="E2688">
+        <v>171156</v>
+      </c>
+      <c r="F2688" s="26">
+        <f t="shared" si="226"/>
+        <v>11257</v>
+      </c>
+      <c r="G2688" s="19">
+        <f t="shared" si="230"/>
+        <v>1566</v>
+      </c>
+      <c r="H2688" s="15">
+        <f t="shared" si="231"/>
+        <v>43</v>
+      </c>
+      <c r="I2688" s="23">
+        <f t="shared" si="232"/>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2689" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2689" s="8">
+        <v>44270</v>
+      </c>
+      <c r="C2689">
+        <v>261582</v>
+      </c>
+      <c r="D2689">
+        <v>4461</v>
+      </c>
+      <c r="E2689">
+        <v>252857</v>
+      </c>
+      <c r="F2689" s="26">
+        <f t="shared" si="226"/>
+        <v>4264</v>
+      </c>
+      <c r="G2689" s="19">
+        <f t="shared" si="230"/>
+        <v>171</v>
+      </c>
+      <c r="H2689" s="15">
+        <f t="shared" si="231"/>
+        <v>3</v>
+      </c>
+      <c r="I2689" s="23">
+        <f t="shared" si="232"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2690" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2690" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2691" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2691" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2692" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2692" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2693" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2693" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2694" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2694" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2695" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2695" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2696" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2696" s="8">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1048576" s="8">
+        <v>44269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
covid-19 march 18 update
</commit_message>
<xml_diff>
--- a/COVID-19_DATA.xlsx
+++ b/COVID-19_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="16">
   <si>
     <t>Cumulative  Test positive</t>
   </si>
@@ -1003,10 +1003,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2678" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2695" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2690" sqref="C2690"/>
+      <selection pane="bottomRight" activeCell="G2697" sqref="G2697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88827,7 +88827,7 @@
         <v>9808</v>
       </c>
       <c r="F2662" s="26">
-        <f t="shared" ref="F2662:F2689" si="226">C2662-D2662-E2662</f>
+        <f t="shared" ref="F2662:F2696" si="226">C2662-D2662-E2662</f>
         <v>767</v>
       </c>
       <c r="G2662" s="19">
@@ -89741,6 +89741,31 @@
       <c r="B2690" s="8">
         <v>44271</v>
       </c>
+      <c r="C2690">
+        <v>11161</v>
+      </c>
+      <c r="D2690">
+        <v>322</v>
+      </c>
+      <c r="E2690">
+        <v>10045</v>
+      </c>
+      <c r="F2690" s="26">
+        <f t="shared" si="226"/>
+        <v>794</v>
+      </c>
+      <c r="G2690" s="19">
+        <f t="shared" ref="G2690:G2696" si="233">C2690-C2683</f>
+        <v>72</v>
+      </c>
+      <c r="H2690" s="15">
+        <f t="shared" ref="H2690:H2696" si="234">D2690-D2683</f>
+        <v>0</v>
+      </c>
+      <c r="I2690" s="23">
+        <f t="shared" ref="I2690:I2696" si="235">E2690-E2683</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="2691" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2691" s="11" t="s">
@@ -89749,6 +89774,31 @@
       <c r="B2691" s="8">
         <v>44271</v>
       </c>
+      <c r="C2691">
+        <v>19247</v>
+      </c>
+      <c r="D2691">
+        <v>202</v>
+      </c>
+      <c r="E2691">
+        <v>18896</v>
+      </c>
+      <c r="F2691" s="26">
+        <f t="shared" si="226"/>
+        <v>149</v>
+      </c>
+      <c r="G2691" s="19">
+        <f t="shared" si="233"/>
+        <v>14</v>
+      </c>
+      <c r="H2691" s="15">
+        <f t="shared" si="234"/>
+        <v>0</v>
+      </c>
+      <c r="I2691" s="23">
+        <f t="shared" si="235"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="2692" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2692" s="11" t="s">
@@ -89757,6 +89807,31 @@
       <c r="B2692" s="8">
         <v>44271</v>
       </c>
+      <c r="C2692">
+        <v>4965</v>
+      </c>
+      <c r="D2692">
+        <v>103</v>
+      </c>
+      <c r="E2692">
+        <v>4856</v>
+      </c>
+      <c r="F2692" s="26">
+        <f t="shared" si="226"/>
+        <v>6</v>
+      </c>
+      <c r="G2692" s="19">
+        <f t="shared" si="233"/>
+        <v>4</v>
+      </c>
+      <c r="H2692" s="15">
+        <f t="shared" si="234"/>
+        <v>0</v>
+      </c>
+      <c r="I2692" s="23">
+        <f t="shared" si="235"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="2693" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2693" s="11" t="s">
@@ -89765,6 +89840,31 @@
       <c r="B2693" s="8">
         <v>44271</v>
       </c>
+      <c r="C2693">
+        <v>48938</v>
+      </c>
+      <c r="D2693">
+        <v>529</v>
+      </c>
+      <c r="E2693">
+        <v>44636</v>
+      </c>
+      <c r="F2693" s="26">
+        <f t="shared" si="226"/>
+        <v>3773</v>
+      </c>
+      <c r="G2693" s="19">
+        <f t="shared" si="233"/>
+        <v>443</v>
+      </c>
+      <c r="H2693" s="15">
+        <f t="shared" si="234"/>
+        <v>3</v>
+      </c>
+      <c r="I2693" s="23">
+        <f t="shared" si="235"/>
+        <v>227</v>
+      </c>
     </row>
     <row r="2694" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2694" s="11" t="s">
@@ -89773,6 +89873,31 @@
       <c r="B2694" s="8">
         <v>44271</v>
       </c>
+      <c r="C2694">
+        <v>76819</v>
+      </c>
+      <c r="D2694">
+        <v>2179</v>
+      </c>
+      <c r="E2694">
+        <v>71104</v>
+      </c>
+      <c r="F2694" s="26">
+        <f t="shared" si="226"/>
+        <v>3536</v>
+      </c>
+      <c r="G2694" s="19">
+        <f t="shared" si="233"/>
+        <v>440</v>
+      </c>
+      <c r="H2694" s="15">
+        <f t="shared" si="234"/>
+        <v>10</v>
+      </c>
+      <c r="I2694" s="23">
+        <f t="shared" si="235"/>
+        <v>243</v>
+      </c>
     </row>
     <row r="2695" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2695" s="11" t="s">
@@ -89781,6 +89906,31 @@
       <c r="B2695" s="8">
         <v>44271</v>
       </c>
+      <c r="C2695">
+        <v>189362</v>
+      </c>
+      <c r="D2695">
+        <v>5853</v>
+      </c>
+      <c r="E2695">
+        <v>173289</v>
+      </c>
+      <c r="F2695" s="26">
+        <f t="shared" si="226"/>
+        <v>10220</v>
+      </c>
+      <c r="G2695" s="19">
+        <f t="shared" si="233"/>
+        <v>1137</v>
+      </c>
+      <c r="H2695" s="15">
+        <f t="shared" si="234"/>
+        <v>41</v>
+      </c>
+      <c r="I2695" s="23">
+        <f t="shared" si="235"/>
+        <v>2133</v>
+      </c>
     </row>
     <row r="2696" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2696" s="11" t="s">
@@ -89788,6 +89938,493 @@
       </c>
       <c r="B2696" s="8">
         <v>44271</v>
+      </c>
+      <c r="C2696">
+        <v>261823</v>
+      </c>
+      <c r="D2696">
+        <v>4468</v>
+      </c>
+      <c r="E2696">
+        <v>253041</v>
+      </c>
+      <c r="F2696" s="26">
+        <f t="shared" si="226"/>
+        <v>4314</v>
+      </c>
+      <c r="G2696" s="19">
+        <f t="shared" si="233"/>
+        <v>241</v>
+      </c>
+      <c r="H2696" s="15">
+        <f t="shared" si="234"/>
+        <v>7</v>
+      </c>
+      <c r="I2696" s="23">
+        <f t="shared" si="235"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2697" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2697" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2697">
+        <v>11264</v>
+      </c>
+      <c r="D2697">
+        <v>328</v>
+      </c>
+      <c r="E2697">
+        <v>10106</v>
+      </c>
+      <c r="F2697" s="26">
+        <f t="shared" ref="F2697:F2710" si="236">C2697-D2697-E2697</f>
+        <v>830</v>
+      </c>
+      <c r="G2697" s="19">
+        <f t="shared" ref="G2697:G2710" si="237">C2697-C2690</f>
+        <v>103</v>
+      </c>
+      <c r="H2697" s="15">
+        <f t="shared" ref="H2697:H2710" si="238">D2697-D2690</f>
+        <v>6</v>
+      </c>
+      <c r="I2697" s="23">
+        <f t="shared" ref="I2697:I2710" si="239">E2697-E2690</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2698" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2698" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2698">
+        <v>19269</v>
+      </c>
+      <c r="D2698">
+        <v>202</v>
+      </c>
+      <c r="E2698">
+        <v>18908</v>
+      </c>
+      <c r="F2698" s="26">
+        <f t="shared" si="236"/>
+        <v>159</v>
+      </c>
+      <c r="G2698" s="19">
+        <f t="shared" si="237"/>
+        <v>22</v>
+      </c>
+      <c r="H2698" s="15">
+        <f t="shared" si="238"/>
+        <v>0</v>
+      </c>
+      <c r="I2698" s="23">
+        <f t="shared" si="239"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2699" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2699" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2699">
+        <v>4965</v>
+      </c>
+      <c r="D2699">
+        <v>103</v>
+      </c>
+      <c r="E2699">
+        <v>4856</v>
+      </c>
+      <c r="F2699" s="26">
+        <f t="shared" si="236"/>
+        <v>6</v>
+      </c>
+      <c r="G2699" s="19">
+        <f t="shared" si="237"/>
+        <v>0</v>
+      </c>
+      <c r="H2699" s="15">
+        <f t="shared" si="238"/>
+        <v>0</v>
+      </c>
+      <c r="I2699" s="23">
+        <f t="shared" si="239"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2700" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2700" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2700">
+        <v>49476</v>
+      </c>
+      <c r="D2700">
+        <v>531</v>
+      </c>
+      <c r="E2700">
+        <v>44828</v>
+      </c>
+      <c r="F2700" s="26">
+        <f t="shared" si="236"/>
+        <v>4117</v>
+      </c>
+      <c r="G2700" s="19">
+        <f t="shared" si="237"/>
+        <v>538</v>
+      </c>
+      <c r="H2700" s="15">
+        <f t="shared" si="238"/>
+        <v>2</v>
+      </c>
+      <c r="I2700" s="23">
+        <f t="shared" si="239"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2701" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2701" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2701">
+        <v>77443</v>
+      </c>
+      <c r="D2701">
+        <v>2188</v>
+      </c>
+      <c r="E2701">
+        <v>71297</v>
+      </c>
+      <c r="F2701" s="26">
+        <f t="shared" si="236"/>
+        <v>3958</v>
+      </c>
+      <c r="G2701" s="19">
+        <f t="shared" si="237"/>
+        <v>624</v>
+      </c>
+      <c r="H2701" s="15">
+        <f t="shared" si="238"/>
+        <v>9</v>
+      </c>
+      <c r="I2701" s="23">
+        <f t="shared" si="239"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2702" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2702" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2702">
+        <v>191186</v>
+      </c>
+      <c r="D2702">
+        <v>5896</v>
+      </c>
+      <c r="E2702">
+        <v>174269</v>
+      </c>
+      <c r="F2702" s="26">
+        <f t="shared" si="236"/>
+        <v>11021</v>
+      </c>
+      <c r="G2702" s="19">
+        <f t="shared" si="237"/>
+        <v>1824</v>
+      </c>
+      <c r="H2702" s="15">
+        <f t="shared" si="238"/>
+        <v>43</v>
+      </c>
+      <c r="I2702" s="23">
+        <f t="shared" si="239"/>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2703" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2703" s="8">
+        <v>44272</v>
+      </c>
+      <c r="C2703">
+        <v>262207</v>
+      </c>
+      <c r="D2703">
+        <v>4469</v>
+      </c>
+      <c r="E2703">
+        <v>253237</v>
+      </c>
+      <c r="F2703" s="26">
+        <f t="shared" si="236"/>
+        <v>4501</v>
+      </c>
+      <c r="G2703" s="19">
+        <f t="shared" si="237"/>
+        <v>384</v>
+      </c>
+      <c r="H2703" s="15">
+        <f t="shared" si="238"/>
+        <v>1</v>
+      </c>
+      <c r="I2703" s="23">
+        <f t="shared" si="239"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2704" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2704" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2704">
+        <v>11377</v>
+      </c>
+      <c r="D2704">
+        <v>328</v>
+      </c>
+      <c r="E2704">
+        <v>10178</v>
+      </c>
+      <c r="F2704" s="26">
+        <f t="shared" si="236"/>
+        <v>871</v>
+      </c>
+      <c r="G2704" s="19">
+        <f t="shared" si="237"/>
+        <v>113</v>
+      </c>
+      <c r="H2704" s="15">
+        <f t="shared" si="238"/>
+        <v>0</v>
+      </c>
+      <c r="I2704" s="23">
+        <f t="shared" si="239"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2705" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2705" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2705">
+        <v>19290</v>
+      </c>
+      <c r="D2705">
+        <v>202</v>
+      </c>
+      <c r="E2705">
+        <v>18910</v>
+      </c>
+      <c r="F2705" s="26">
+        <f t="shared" si="236"/>
+        <v>178</v>
+      </c>
+      <c r="G2705" s="19">
+        <f t="shared" si="237"/>
+        <v>21</v>
+      </c>
+      <c r="H2705" s="15">
+        <f t="shared" si="238"/>
+        <v>0</v>
+      </c>
+      <c r="I2705" s="23">
+        <f t="shared" si="239"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2706" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2706" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2706">
+        <v>4967</v>
+      </c>
+      <c r="D2706">
+        <v>103</v>
+      </c>
+      <c r="E2706">
+        <v>4856</v>
+      </c>
+      <c r="F2706" s="26">
+        <f t="shared" si="236"/>
+        <v>8</v>
+      </c>
+      <c r="G2706" s="19">
+        <f t="shared" si="237"/>
+        <v>2</v>
+      </c>
+      <c r="H2706" s="15">
+        <f t="shared" si="238"/>
+        <v>0</v>
+      </c>
+      <c r="I2706" s="23">
+        <f t="shared" si="239"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2707" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2707" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2707">
+        <v>50096</v>
+      </c>
+      <c r="D2707">
+        <v>536</v>
+      </c>
+      <c r="E2707">
+        <v>44976</v>
+      </c>
+      <c r="F2707" s="26">
+        <f t="shared" si="236"/>
+        <v>4584</v>
+      </c>
+      <c r="G2707" s="19">
+        <f t="shared" si="237"/>
+        <v>620</v>
+      </c>
+      <c r="H2707" s="15">
+        <f t="shared" si="238"/>
+        <v>5</v>
+      </c>
+      <c r="I2707" s="23">
+        <f t="shared" si="239"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2708" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2708" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2708">
+        <v>77972</v>
+      </c>
+      <c r="D2708">
+        <v>2196</v>
+      </c>
+      <c r="E2708">
+        <v>71518</v>
+      </c>
+      <c r="F2708" s="26">
+        <f t="shared" si="236"/>
+        <v>4258</v>
+      </c>
+      <c r="G2708" s="19">
+        <f t="shared" si="237"/>
+        <v>529</v>
+      </c>
+      <c r="H2708" s="15">
+        <f t="shared" si="238"/>
+        <v>8</v>
+      </c>
+      <c r="I2708" s="23">
+        <f t="shared" si="239"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2709" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2709" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2709">
+        <v>193054</v>
+      </c>
+      <c r="D2709">
+        <v>5919</v>
+      </c>
+      <c r="E2709">
+        <v>174566</v>
+      </c>
+      <c r="F2709" s="26">
+        <f t="shared" si="236"/>
+        <v>12569</v>
+      </c>
+      <c r="G2709" s="19">
+        <f t="shared" si="237"/>
+        <v>1868</v>
+      </c>
+      <c r="H2709" s="15">
+        <f t="shared" si="238"/>
+        <v>23</v>
+      </c>
+      <c r="I2709" s="23">
+        <f t="shared" si="239"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2710" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2710" s="8">
+        <v>44273</v>
+      </c>
+      <c r="C2710">
+        <v>262503</v>
+      </c>
+      <c r="D2710">
+        <v>4473</v>
+      </c>
+      <c r="E2710">
+        <v>253310</v>
+      </c>
+      <c r="F2710" s="26">
+        <f t="shared" si="236"/>
+        <v>4720</v>
+      </c>
+      <c r="G2710" s="19">
+        <f t="shared" si="237"/>
+        <v>296</v>
+      </c>
+      <c r="H2710" s="15">
+        <f t="shared" si="238"/>
+        <v>4</v>
+      </c>
+      <c r="I2710" s="23">
+        <f t="shared" si="239"/>
+        <v>73</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update march 31, 2021
</commit_message>
<xml_diff>
--- a/COVID-19_DATA.xlsx
+++ b/COVID-19_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="16">
   <si>
     <t>Cumulative  Test positive</t>
   </si>
@@ -1003,10 +1003,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2695" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2793" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2697" sqref="G2697"/>
+      <selection pane="bottomRight" activeCell="F2796" sqref="F2796"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -90427,6 +90427,2778 @@
         <v>73</v>
       </c>
     </row>
+    <row r="2711" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2711" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2711" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2711">
+        <v>11483</v>
+      </c>
+      <c r="D2711">
+        <v>330</v>
+      </c>
+      <c r="E2711">
+        <v>10242</v>
+      </c>
+      <c r="F2711" s="26">
+        <f t="shared" ref="F2711:F2774" si="240">C2711-D2711-E2711</f>
+        <v>911</v>
+      </c>
+      <c r="G2711" s="19">
+        <f t="shared" ref="G2711:G2774" si="241">C2711-C2704</f>
+        <v>106</v>
+      </c>
+      <c r="H2711" s="15">
+        <f t="shared" ref="H2711:H2774" si="242">D2711-D2704</f>
+        <v>2</v>
+      </c>
+      <c r="I2711" s="23">
+        <f t="shared" ref="I2711:I2774" si="243">E2711-E2704</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2712" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2712" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2712">
+        <v>19306</v>
+      </c>
+      <c r="D2712">
+        <v>203</v>
+      </c>
+      <c r="E2712">
+        <v>18919</v>
+      </c>
+      <c r="F2712" s="26">
+        <f t="shared" si="240"/>
+        <v>184</v>
+      </c>
+      <c r="G2712" s="19">
+        <f t="shared" si="241"/>
+        <v>16</v>
+      </c>
+      <c r="H2712" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2712" s="23">
+        <f t="shared" si="243"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2713" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2713" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2713">
+        <v>4967</v>
+      </c>
+      <c r="D2713">
+        <v>103</v>
+      </c>
+      <c r="E2713">
+        <v>4856</v>
+      </c>
+      <c r="F2713" s="26">
+        <f t="shared" si="240"/>
+        <v>8</v>
+      </c>
+      <c r="G2713" s="19">
+        <f t="shared" si="241"/>
+        <v>0</v>
+      </c>
+      <c r="H2713" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2713" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2714" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2714" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2714">
+        <v>50843</v>
+      </c>
+      <c r="D2714">
+        <v>539</v>
+      </c>
+      <c r="E2714">
+        <v>45161</v>
+      </c>
+      <c r="F2714" s="26">
+        <f t="shared" si="240"/>
+        <v>5143</v>
+      </c>
+      <c r="G2714" s="19">
+        <f t="shared" si="241"/>
+        <v>747</v>
+      </c>
+      <c r="H2714" s="15">
+        <f t="shared" si="242"/>
+        <v>3</v>
+      </c>
+      <c r="I2714" s="23">
+        <f t="shared" si="243"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2715" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2715" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2715">
+        <v>78653</v>
+      </c>
+      <c r="D2715">
+        <v>2202</v>
+      </c>
+      <c r="E2715">
+        <v>71861</v>
+      </c>
+      <c r="F2715" s="26">
+        <f t="shared" si="240"/>
+        <v>4590</v>
+      </c>
+      <c r="G2715" s="19">
+        <f t="shared" si="241"/>
+        <v>681</v>
+      </c>
+      <c r="H2715" s="15">
+        <f t="shared" si="242"/>
+        <v>6</v>
+      </c>
+      <c r="I2715" s="23">
+        <f t="shared" si="243"/>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2716" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2716" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2716">
+        <v>195087</v>
+      </c>
+      <c r="D2716">
+        <v>5944</v>
+      </c>
+      <c r="E2716">
+        <v>175265</v>
+      </c>
+      <c r="F2716" s="26">
+        <f t="shared" si="240"/>
+        <v>13878</v>
+      </c>
+      <c r="G2716" s="19">
+        <f t="shared" si="241"/>
+        <v>2033</v>
+      </c>
+      <c r="H2716" s="15">
+        <f t="shared" si="242"/>
+        <v>25</v>
+      </c>
+      <c r="I2716" s="23">
+        <f t="shared" si="243"/>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2717" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2717" s="8">
+        <v>44274</v>
+      </c>
+      <c r="C2717">
+        <v>262796</v>
+      </c>
+      <c r="D2717">
+        <v>4478</v>
+      </c>
+      <c r="E2717">
+        <v>253456</v>
+      </c>
+      <c r="F2717" s="26">
+        <f t="shared" si="240"/>
+        <v>4862</v>
+      </c>
+      <c r="G2717" s="19">
+        <f t="shared" si="241"/>
+        <v>293</v>
+      </c>
+      <c r="H2717" s="15">
+        <f t="shared" si="242"/>
+        <v>5</v>
+      </c>
+      <c r="I2717" s="23">
+        <f t="shared" si="243"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2718" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2718" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2718">
+        <v>11609</v>
+      </c>
+      <c r="D2718">
+        <v>333</v>
+      </c>
+      <c r="E2718">
+        <v>10296</v>
+      </c>
+      <c r="F2718" s="26">
+        <f t="shared" si="240"/>
+        <v>980</v>
+      </c>
+      <c r="G2718" s="19">
+        <f t="shared" si="241"/>
+        <v>126</v>
+      </c>
+      <c r="H2718" s="15">
+        <f t="shared" si="242"/>
+        <v>3</v>
+      </c>
+      <c r="I2718" s="23">
+        <f t="shared" si="243"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2719" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2719" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2719">
+        <v>19327</v>
+      </c>
+      <c r="D2719">
+        <v>203</v>
+      </c>
+      <c r="E2719">
+        <v>18925</v>
+      </c>
+      <c r="F2719" s="26">
+        <f t="shared" si="240"/>
+        <v>199</v>
+      </c>
+      <c r="G2719" s="19">
+        <f t="shared" si="241"/>
+        <v>21</v>
+      </c>
+      <c r="H2719" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2719" s="23">
+        <f t="shared" si="243"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2720" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2720" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2720">
+        <v>4972</v>
+      </c>
+      <c r="D2720">
+        <v>103</v>
+      </c>
+      <c r="E2720">
+        <v>4856</v>
+      </c>
+      <c r="F2720" s="26">
+        <f t="shared" si="240"/>
+        <v>13</v>
+      </c>
+      <c r="G2720" s="19">
+        <f t="shared" si="241"/>
+        <v>5</v>
+      </c>
+      <c r="H2720" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2720" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2721" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2721" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2721">
+        <v>51414</v>
+      </c>
+      <c r="D2721">
+        <v>543</v>
+      </c>
+      <c r="E2721">
+        <v>45381</v>
+      </c>
+      <c r="F2721" s="26">
+        <f t="shared" si="240"/>
+        <v>5490</v>
+      </c>
+      <c r="G2721" s="19">
+        <f t="shared" si="241"/>
+        <v>571</v>
+      </c>
+      <c r="H2721" s="15">
+        <f t="shared" si="242"/>
+        <v>4</v>
+      </c>
+      <c r="I2721" s="23">
+        <f t="shared" si="243"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2722" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2722" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2722">
+        <v>79245</v>
+      </c>
+      <c r="D2722">
+        <v>2208</v>
+      </c>
+      <c r="E2722">
+        <v>72111</v>
+      </c>
+      <c r="F2722" s="26">
+        <f t="shared" si="240"/>
+        <v>4926</v>
+      </c>
+      <c r="G2722" s="19">
+        <f t="shared" si="241"/>
+        <v>592</v>
+      </c>
+      <c r="H2722" s="15">
+        <f t="shared" si="242"/>
+        <v>6</v>
+      </c>
+      <c r="I2722" s="23">
+        <f t="shared" si="243"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2723" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2723" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2723">
+        <v>197177</v>
+      </c>
+      <c r="D2723">
+        <v>5974</v>
+      </c>
+      <c r="E2723">
+        <v>176699</v>
+      </c>
+      <c r="F2723" s="26">
+        <f t="shared" si="240"/>
+        <v>14504</v>
+      </c>
+      <c r="G2723" s="19">
+        <f t="shared" si="241"/>
+        <v>2090</v>
+      </c>
+      <c r="H2723" s="15">
+        <f t="shared" si="242"/>
+        <v>30</v>
+      </c>
+      <c r="I2723" s="23">
+        <f t="shared" si="243"/>
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2724" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2724" s="8">
+        <v>44275</v>
+      </c>
+      <c r="C2724">
+        <v>263058</v>
+      </c>
+      <c r="D2724">
+        <v>4479</v>
+      </c>
+      <c r="E2724">
+        <v>253584</v>
+      </c>
+      <c r="F2724" s="26">
+        <f t="shared" si="240"/>
+        <v>4995</v>
+      </c>
+      <c r="G2724" s="19">
+        <f t="shared" si="241"/>
+        <v>262</v>
+      </c>
+      <c r="H2724" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2724" s="23">
+        <f t="shared" si="243"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2725" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2725" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2725">
+        <v>11704</v>
+      </c>
+      <c r="D2725">
+        <v>336</v>
+      </c>
+      <c r="E2725">
+        <v>10355</v>
+      </c>
+      <c r="F2725" s="26">
+        <f t="shared" si="240"/>
+        <v>1013</v>
+      </c>
+      <c r="G2725" s="19">
+        <f t="shared" si="241"/>
+        <v>95</v>
+      </c>
+      <c r="H2725" s="15">
+        <f t="shared" si="242"/>
+        <v>3</v>
+      </c>
+      <c r="I2725" s="23">
+        <f t="shared" si="243"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2726" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2726" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2726">
+        <v>19342</v>
+      </c>
+      <c r="D2726">
+        <v>203</v>
+      </c>
+      <c r="E2726">
+        <v>18941</v>
+      </c>
+      <c r="F2726" s="26">
+        <f t="shared" si="240"/>
+        <v>198</v>
+      </c>
+      <c r="G2726" s="19">
+        <f t="shared" si="241"/>
+        <v>15</v>
+      </c>
+      <c r="H2726" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2726" s="23">
+        <f t="shared" si="243"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2727" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2727" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2727">
+        <v>4972</v>
+      </c>
+      <c r="D2727">
+        <v>103</v>
+      </c>
+      <c r="E2727">
+        <v>4856</v>
+      </c>
+      <c r="F2727" s="26">
+        <f t="shared" si="240"/>
+        <v>13</v>
+      </c>
+      <c r="G2727" s="19">
+        <f t="shared" si="241"/>
+        <v>0</v>
+      </c>
+      <c r="H2727" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2727" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2728" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2728" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2728">
+        <v>52086</v>
+      </c>
+      <c r="D2728">
+        <v>545</v>
+      </c>
+      <c r="E2728">
+        <v>45636</v>
+      </c>
+      <c r="F2728" s="26">
+        <f t="shared" si="240"/>
+        <v>5905</v>
+      </c>
+      <c r="G2728" s="19">
+        <f t="shared" si="241"/>
+        <v>672</v>
+      </c>
+      <c r="H2728" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2728" s="23">
+        <f t="shared" si="243"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2729" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2729" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2729">
+        <v>80037</v>
+      </c>
+      <c r="D2729">
+        <v>2215</v>
+      </c>
+      <c r="E2729">
+        <v>72322</v>
+      </c>
+      <c r="F2729" s="26">
+        <f t="shared" si="240"/>
+        <v>5500</v>
+      </c>
+      <c r="G2729" s="19">
+        <f t="shared" si="241"/>
+        <v>792</v>
+      </c>
+      <c r="H2729" s="15">
+        <f t="shared" si="242"/>
+        <v>7</v>
+      </c>
+      <c r="I2729" s="23">
+        <f t="shared" si="243"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2730" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2730" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2730">
+        <v>199040</v>
+      </c>
+      <c r="D2730">
+        <v>5982</v>
+      </c>
+      <c r="E2730">
+        <v>177698</v>
+      </c>
+      <c r="F2730" s="26">
+        <f t="shared" si="240"/>
+        <v>15360</v>
+      </c>
+      <c r="G2730" s="19">
+        <f t="shared" si="241"/>
+        <v>1863</v>
+      </c>
+      <c r="H2730" s="15">
+        <f t="shared" si="242"/>
+        <v>8</v>
+      </c>
+      <c r="I2730" s="23">
+        <f t="shared" si="243"/>
+        <v>999</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2731" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2731" s="8">
+        <v>44276</v>
+      </c>
+      <c r="C2731">
+        <v>263290</v>
+      </c>
+      <c r="D2731">
+        <v>4479</v>
+      </c>
+      <c r="E2731">
+        <v>253730</v>
+      </c>
+      <c r="F2731" s="26">
+        <f t="shared" si="240"/>
+        <v>5081</v>
+      </c>
+      <c r="G2731" s="19">
+        <f t="shared" si="241"/>
+        <v>232</v>
+      </c>
+      <c r="H2731" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2731" s="23">
+        <f t="shared" si="243"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2732" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2732" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2732">
+        <v>11792</v>
+      </c>
+      <c r="D2732">
+        <v>338</v>
+      </c>
+      <c r="E2732">
+        <v>10406</v>
+      </c>
+      <c r="F2732" s="26">
+        <f t="shared" si="240"/>
+        <v>1048</v>
+      </c>
+      <c r="G2732" s="19">
+        <f t="shared" si="241"/>
+        <v>88</v>
+      </c>
+      <c r="H2732" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2732" s="23">
+        <f t="shared" si="243"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2733" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2733" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2733">
+        <v>19347</v>
+      </c>
+      <c r="D2733">
+        <v>203</v>
+      </c>
+      <c r="E2733">
+        <v>18958</v>
+      </c>
+      <c r="F2733" s="26">
+        <f t="shared" si="240"/>
+        <v>186</v>
+      </c>
+      <c r="G2733" s="19">
+        <f t="shared" si="241"/>
+        <v>5</v>
+      </c>
+      <c r="H2733" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2733" s="23">
+        <f t="shared" si="243"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2734" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2734" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2734">
+        <v>4974</v>
+      </c>
+      <c r="D2734">
+        <v>103</v>
+      </c>
+      <c r="E2734">
+        <v>4856</v>
+      </c>
+      <c r="F2734" s="26">
+        <f t="shared" si="240"/>
+        <v>15</v>
+      </c>
+      <c r="G2734" s="19">
+        <f t="shared" si="241"/>
+        <v>2</v>
+      </c>
+      <c r="H2734" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2734" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2735" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2735" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2735">
+        <v>52676</v>
+      </c>
+      <c r="D2735">
+        <v>548</v>
+      </c>
+      <c r="E2735">
+        <v>45818</v>
+      </c>
+      <c r="F2735" s="26">
+        <f t="shared" si="240"/>
+        <v>6310</v>
+      </c>
+      <c r="G2735" s="19">
+        <f t="shared" si="241"/>
+        <v>590</v>
+      </c>
+      <c r="H2735" s="15">
+        <f t="shared" si="242"/>
+        <v>3</v>
+      </c>
+      <c r="I2735" s="23">
+        <f t="shared" si="243"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2736" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2736" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2736">
+        <v>80519</v>
+      </c>
+      <c r="D2736">
+        <v>2225</v>
+      </c>
+      <c r="E2736">
+        <v>72500</v>
+      </c>
+      <c r="F2736" s="26">
+        <f t="shared" si="240"/>
+        <v>5794</v>
+      </c>
+      <c r="G2736" s="19">
+        <f t="shared" si="241"/>
+        <v>482</v>
+      </c>
+      <c r="H2736" s="15">
+        <f t="shared" si="242"/>
+        <v>10</v>
+      </c>
+      <c r="I2736" s="23">
+        <f t="shared" si="243"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2737" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2737" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2737">
+        <v>200969</v>
+      </c>
+      <c r="D2737">
+        <v>6039</v>
+      </c>
+      <c r="E2737">
+        <v>178898</v>
+      </c>
+      <c r="F2737" s="26">
+        <f t="shared" si="240"/>
+        <v>16032</v>
+      </c>
+      <c r="G2737" s="19">
+        <f t="shared" si="241"/>
+        <v>1929</v>
+      </c>
+      <c r="H2737" s="15">
+        <f t="shared" si="242"/>
+        <v>57</v>
+      </c>
+      <c r="I2737" s="23">
+        <f t="shared" si="243"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2738" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2738" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C2738">
+        <v>263464</v>
+      </c>
+      <c r="D2738">
+        <v>4479</v>
+      </c>
+      <c r="E2738">
+        <v>253835</v>
+      </c>
+      <c r="F2738" s="26">
+        <f t="shared" si="240"/>
+        <v>5150</v>
+      </c>
+      <c r="G2738" s="19">
+        <f t="shared" si="241"/>
+        <v>174</v>
+      </c>
+      <c r="H2738" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2738" s="23">
+        <f t="shared" si="243"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2739" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2739" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2739">
+        <v>11946</v>
+      </c>
+      <c r="D2739">
+        <v>339</v>
+      </c>
+      <c r="E2739">
+        <v>10459</v>
+      </c>
+      <c r="F2739" s="26">
+        <f t="shared" si="240"/>
+        <v>1148</v>
+      </c>
+      <c r="G2739" s="19">
+        <f t="shared" si="241"/>
+        <v>154</v>
+      </c>
+      <c r="H2739" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2739" s="23">
+        <f t="shared" si="243"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2740" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2740" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2740">
+        <v>19374</v>
+      </c>
+      <c r="D2740">
+        <v>203</v>
+      </c>
+      <c r="E2740">
+        <v>18975</v>
+      </c>
+      <c r="F2740" s="26">
+        <f t="shared" si="240"/>
+        <v>196</v>
+      </c>
+      <c r="G2740" s="19">
+        <f t="shared" si="241"/>
+        <v>27</v>
+      </c>
+      <c r="H2740" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2740" s="23">
+        <f t="shared" si="243"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2741" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2741" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2741">
+        <v>4975</v>
+      </c>
+      <c r="D2741">
+        <v>103</v>
+      </c>
+      <c r="E2741">
+        <v>4856</v>
+      </c>
+      <c r="F2741" s="26">
+        <f t="shared" si="240"/>
+        <v>16</v>
+      </c>
+      <c r="G2741" s="19">
+        <f t="shared" si="241"/>
+        <v>1</v>
+      </c>
+      <c r="H2741" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2741" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2742" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2742" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2742">
+        <v>53136</v>
+      </c>
+      <c r="D2742">
+        <v>552</v>
+      </c>
+      <c r="E2742">
+        <v>46067</v>
+      </c>
+      <c r="F2742" s="26">
+        <f t="shared" si="240"/>
+        <v>6517</v>
+      </c>
+      <c r="G2742" s="19">
+        <f t="shared" si="241"/>
+        <v>460</v>
+      </c>
+      <c r="H2742" s="15">
+        <f t="shared" si="242"/>
+        <v>4</v>
+      </c>
+      <c r="I2742" s="23">
+        <f t="shared" si="243"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2743" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2743" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2743">
+        <v>81204</v>
+      </c>
+      <c r="D2743">
+        <v>2238</v>
+      </c>
+      <c r="E2743">
+        <v>72948</v>
+      </c>
+      <c r="F2743" s="26">
+        <f t="shared" si="240"/>
+        <v>6018</v>
+      </c>
+      <c r="G2743" s="19">
+        <f t="shared" si="241"/>
+        <v>685</v>
+      </c>
+      <c r="H2743" s="15">
+        <f t="shared" si="242"/>
+        <v>13</v>
+      </c>
+      <c r="I2743" s="23">
+        <f t="shared" si="243"/>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2744" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2744" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2744">
+        <v>202743</v>
+      </c>
+      <c r="D2744">
+        <v>6048</v>
+      </c>
+      <c r="E2744">
+        <v>178942</v>
+      </c>
+      <c r="F2744" s="26">
+        <f t="shared" si="240"/>
+        <v>17753</v>
+      </c>
+      <c r="G2744" s="19">
+        <f t="shared" si="241"/>
+        <v>1774</v>
+      </c>
+      <c r="H2744" s="15">
+        <f t="shared" si="242"/>
+        <v>9</v>
+      </c>
+      <c r="I2744" s="23">
+        <f t="shared" si="243"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2745" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2745" s="8">
+        <v>44278</v>
+      </c>
+      <c r="C2745">
+        <v>263664</v>
+      </c>
+      <c r="D2745">
+        <v>4482</v>
+      </c>
+      <c r="E2745">
+        <v>253981</v>
+      </c>
+      <c r="F2745" s="26">
+        <f t="shared" si="240"/>
+        <v>5201</v>
+      </c>
+      <c r="G2745" s="19">
+        <f t="shared" si="241"/>
+        <v>200</v>
+      </c>
+      <c r="H2745" s="15">
+        <f t="shared" si="242"/>
+        <v>3</v>
+      </c>
+      <c r="I2745" s="23">
+        <f t="shared" si="243"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2746" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2746" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2746">
+        <v>12016</v>
+      </c>
+      <c r="D2746">
+        <v>339</v>
+      </c>
+      <c r="E2746">
+        <v>10511</v>
+      </c>
+      <c r="F2746" s="26">
+        <f t="shared" si="240"/>
+        <v>1166</v>
+      </c>
+      <c r="G2746" s="19">
+        <f t="shared" si="241"/>
+        <v>70</v>
+      </c>
+      <c r="H2746" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2746" s="23">
+        <f t="shared" si="243"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2747" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2747" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2747">
+        <v>19395</v>
+      </c>
+      <c r="D2747">
+        <v>205</v>
+      </c>
+      <c r="E2747">
+        <v>18986</v>
+      </c>
+      <c r="F2747" s="26">
+        <f t="shared" si="240"/>
+        <v>204</v>
+      </c>
+      <c r="G2747" s="19">
+        <f t="shared" si="241"/>
+        <v>21</v>
+      </c>
+      <c r="H2747" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2747" s="23">
+        <f t="shared" si="243"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2748" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2748" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2748">
+        <v>4977</v>
+      </c>
+      <c r="D2748">
+        <v>103</v>
+      </c>
+      <c r="E2748">
+        <v>4858</v>
+      </c>
+      <c r="F2748" s="26">
+        <f t="shared" si="240"/>
+        <v>16</v>
+      </c>
+      <c r="G2748" s="19">
+        <f t="shared" si="241"/>
+        <v>2</v>
+      </c>
+      <c r="H2748" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2748" s="23">
+        <f t="shared" si="243"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2749" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2749" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2749">
+        <v>53684</v>
+      </c>
+      <c r="D2749">
+        <v>554</v>
+      </c>
+      <c r="E2749">
+        <v>46307</v>
+      </c>
+      <c r="F2749" s="26">
+        <f t="shared" si="240"/>
+        <v>6823</v>
+      </c>
+      <c r="G2749" s="19">
+        <f t="shared" si="241"/>
+        <v>548</v>
+      </c>
+      <c r="H2749" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2749" s="23">
+        <f t="shared" si="243"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2750" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2750" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2750">
+        <v>81787</v>
+      </c>
+      <c r="D2750">
+        <v>2246</v>
+      </c>
+      <c r="E2750">
+        <v>73171</v>
+      </c>
+      <c r="F2750" s="26">
+        <f t="shared" si="240"/>
+        <v>6370</v>
+      </c>
+      <c r="G2750" s="19">
+        <f t="shared" si="241"/>
+        <v>583</v>
+      </c>
+      <c r="H2750" s="15">
+        <f t="shared" si="242"/>
+        <v>8</v>
+      </c>
+      <c r="I2750" s="23">
+        <f t="shared" si="243"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2751" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2751" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2751">
+        <v>205314</v>
+      </c>
+      <c r="D2751">
+        <v>6099</v>
+      </c>
+      <c r="E2751">
+        <v>179895</v>
+      </c>
+      <c r="F2751" s="26">
+        <f t="shared" si="240"/>
+        <v>19320</v>
+      </c>
+      <c r="G2751" s="19">
+        <f t="shared" si="241"/>
+        <v>2571</v>
+      </c>
+      <c r="H2751" s="15">
+        <f t="shared" si="242"/>
+        <v>51</v>
+      </c>
+      <c r="I2751" s="23">
+        <f t="shared" si="243"/>
+        <v>953</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2752" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2752" s="8">
+        <v>44279</v>
+      </c>
+      <c r="C2752">
+        <v>263815</v>
+      </c>
+      <c r="D2752">
+        <v>4482</v>
+      </c>
+      <c r="E2752">
+        <v>255247</v>
+      </c>
+      <c r="F2752" s="26">
+        <f t="shared" si="240"/>
+        <v>4086</v>
+      </c>
+      <c r="G2752" s="19">
+        <f t="shared" si="241"/>
+        <v>151</v>
+      </c>
+      <c r="H2752" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2752" s="23">
+        <f t="shared" si="243"/>
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2753" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2753" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2753">
+        <v>12095</v>
+      </c>
+      <c r="D2753">
+        <v>340</v>
+      </c>
+      <c r="E2753">
+        <v>10575</v>
+      </c>
+      <c r="F2753" s="26">
+        <f t="shared" si="240"/>
+        <v>1180</v>
+      </c>
+      <c r="G2753" s="19">
+        <f t="shared" si="241"/>
+        <v>79</v>
+      </c>
+      <c r="H2753" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2753" s="23">
+        <f t="shared" si="243"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2754" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2754" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2754">
+        <v>19427</v>
+      </c>
+      <c r="D2754">
+        <v>205</v>
+      </c>
+      <c r="E2754">
+        <v>19003</v>
+      </c>
+      <c r="F2754" s="26">
+        <f t="shared" si="240"/>
+        <v>219</v>
+      </c>
+      <c r="G2754" s="19">
+        <f t="shared" si="241"/>
+        <v>32</v>
+      </c>
+      <c r="H2754" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2754" s="23">
+        <f t="shared" si="243"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2755" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2755" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2755">
+        <v>4983</v>
+      </c>
+      <c r="D2755">
+        <v>103</v>
+      </c>
+      <c r="E2755">
+        <v>4858</v>
+      </c>
+      <c r="F2755" s="26">
+        <f t="shared" si="240"/>
+        <v>22</v>
+      </c>
+      <c r="G2755" s="19">
+        <f t="shared" si="241"/>
+        <v>6</v>
+      </c>
+      <c r="H2755" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2755" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2756" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2756" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2756">
+        <v>54347</v>
+      </c>
+      <c r="D2756">
+        <v>555</v>
+      </c>
+      <c r="E2756">
+        <v>46478</v>
+      </c>
+      <c r="F2756" s="26">
+        <f t="shared" si="240"/>
+        <v>7314</v>
+      </c>
+      <c r="G2756" s="19">
+        <f t="shared" si="241"/>
+        <v>663</v>
+      </c>
+      <c r="H2756" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2756" s="23">
+        <f t="shared" si="243"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2757" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2757" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2757">
+        <v>82677</v>
+      </c>
+      <c r="D2757">
+        <v>2260</v>
+      </c>
+      <c r="E2757">
+        <v>73481</v>
+      </c>
+      <c r="F2757" s="26">
+        <f t="shared" si="240"/>
+        <v>6936</v>
+      </c>
+      <c r="G2757" s="19">
+        <f t="shared" si="241"/>
+        <v>890</v>
+      </c>
+      <c r="H2757" s="15">
+        <f t="shared" si="242"/>
+        <v>14</v>
+      </c>
+      <c r="I2757" s="23">
+        <f t="shared" si="243"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2758" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2758" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2758">
+        <v>207765</v>
+      </c>
+      <c r="D2758">
+        <v>6142</v>
+      </c>
+      <c r="E2758">
+        <v>181351</v>
+      </c>
+      <c r="F2758" s="26">
+        <f t="shared" si="240"/>
+        <v>20272</v>
+      </c>
+      <c r="G2758" s="19">
+        <f t="shared" si="241"/>
+        <v>2451</v>
+      </c>
+      <c r="H2758" s="15">
+        <f t="shared" si="242"/>
+        <v>43</v>
+      </c>
+      <c r="I2758" s="23">
+        <f t="shared" si="243"/>
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2759" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2759" s="8">
+        <v>44280</v>
+      </c>
+      <c r="C2759">
+        <v>264062</v>
+      </c>
+      <c r="D2759">
+        <v>4486</v>
+      </c>
+      <c r="E2759">
+        <v>255399</v>
+      </c>
+      <c r="F2759" s="26">
+        <f t="shared" si="240"/>
+        <v>4177</v>
+      </c>
+      <c r="G2759" s="19">
+        <f t="shared" si="241"/>
+        <v>247</v>
+      </c>
+      <c r="H2759" s="15">
+        <f t="shared" si="242"/>
+        <v>4</v>
+      </c>
+      <c r="I2759" s="23">
+        <f t="shared" si="243"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2760" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2760" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2760">
+        <v>12245</v>
+      </c>
+      <c r="D2760">
+        <v>342</v>
+      </c>
+      <c r="E2760">
+        <v>10631</v>
+      </c>
+      <c r="F2760" s="26">
+        <f t="shared" si="240"/>
+        <v>1272</v>
+      </c>
+      <c r="G2760" s="19">
+        <f t="shared" si="241"/>
+        <v>150</v>
+      </c>
+      <c r="H2760" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2760" s="23">
+        <f t="shared" si="243"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2761" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2761" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2761">
+        <v>19453</v>
+      </c>
+      <c r="D2761">
+        <v>205</v>
+      </c>
+      <c r="E2761">
+        <v>19023</v>
+      </c>
+      <c r="F2761" s="26">
+        <f t="shared" si="240"/>
+        <v>225</v>
+      </c>
+      <c r="G2761" s="19">
+        <f t="shared" si="241"/>
+        <v>26</v>
+      </c>
+      <c r="H2761" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2761" s="23">
+        <f t="shared" si="243"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2762" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2762" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2762">
+        <v>4990</v>
+      </c>
+      <c r="D2762">
+        <v>103</v>
+      </c>
+      <c r="E2762">
+        <v>4858</v>
+      </c>
+      <c r="F2762" s="26">
+        <f t="shared" si="240"/>
+        <v>29</v>
+      </c>
+      <c r="G2762" s="19">
+        <f t="shared" si="241"/>
+        <v>7</v>
+      </c>
+      <c r="H2762" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2762" s="23">
+        <f t="shared" si="243"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2763" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2763" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2763">
+        <v>55056</v>
+      </c>
+      <c r="D2763">
+        <v>557</v>
+      </c>
+      <c r="E2763">
+        <v>46623</v>
+      </c>
+      <c r="F2763" s="26">
+        <f t="shared" si="240"/>
+        <v>7876</v>
+      </c>
+      <c r="G2763" s="19">
+        <f t="shared" si="241"/>
+        <v>709</v>
+      </c>
+      <c r="H2763" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2763" s="23">
+        <f t="shared" si="243"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2764" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2764" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2764">
+        <v>83630</v>
+      </c>
+      <c r="D2764">
+        <v>2274</v>
+      </c>
+      <c r="E2764">
+        <v>74040</v>
+      </c>
+      <c r="F2764" s="26">
+        <f t="shared" si="240"/>
+        <v>7316</v>
+      </c>
+      <c r="G2764" s="19">
+        <f t="shared" si="241"/>
+        <v>953</v>
+      </c>
+      <c r="H2764" s="15">
+        <f t="shared" si="242"/>
+        <v>14</v>
+      </c>
+      <c r="I2764" s="23">
+        <f t="shared" si="243"/>
+        <v>559</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2765" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2765" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2765">
+        <v>210095</v>
+      </c>
+      <c r="D2765">
+        <v>6190</v>
+      </c>
+      <c r="E2765">
+        <v>182596</v>
+      </c>
+      <c r="F2765" s="26">
+        <f t="shared" si="240"/>
+        <v>21309</v>
+      </c>
+      <c r="G2765" s="19">
+        <f t="shared" si="241"/>
+        <v>2330</v>
+      </c>
+      <c r="H2765" s="15">
+        <f t="shared" si="242"/>
+        <v>48</v>
+      </c>
+      <c r="I2765" s="23">
+        <f t="shared" si="243"/>
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2766" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2766" s="8">
+        <v>44281</v>
+      </c>
+      <c r="C2766">
+        <v>264355</v>
+      </c>
+      <c r="D2766">
+        <v>4487</v>
+      </c>
+      <c r="E2766">
+        <v>255511</v>
+      </c>
+      <c r="F2766" s="26">
+        <f t="shared" si="240"/>
+        <v>4357</v>
+      </c>
+      <c r="G2766" s="19">
+        <f t="shared" si="241"/>
+        <v>293</v>
+      </c>
+      <c r="H2766" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2766" s="23">
+        <f t="shared" si="243"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2767" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2767" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2767">
+        <v>12367</v>
+      </c>
+      <c r="D2767">
+        <v>344</v>
+      </c>
+      <c r="E2767">
+        <v>10689</v>
+      </c>
+      <c r="F2767" s="26">
+        <f t="shared" si="240"/>
+        <v>1334</v>
+      </c>
+      <c r="G2767" s="19">
+        <f t="shared" si="241"/>
+        <v>122</v>
+      </c>
+      <c r="H2767" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2767" s="23">
+        <f t="shared" si="243"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2768" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2768" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2768">
+        <v>19497</v>
+      </c>
+      <c r="D2768">
+        <v>206</v>
+      </c>
+      <c r="E2768">
+        <v>19028</v>
+      </c>
+      <c r="F2768" s="26">
+        <f t="shared" si="240"/>
+        <v>263</v>
+      </c>
+      <c r="G2768" s="19">
+        <f t="shared" si="241"/>
+        <v>44</v>
+      </c>
+      <c r="H2768" s="15">
+        <f t="shared" si="242"/>
+        <v>1</v>
+      </c>
+      <c r="I2768" s="23">
+        <f t="shared" si="243"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2769" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2769" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2769">
+        <v>4999</v>
+      </c>
+      <c r="D2769">
+        <v>103</v>
+      </c>
+      <c r="E2769">
+        <v>4859</v>
+      </c>
+      <c r="F2769" s="26">
+        <f t="shared" si="240"/>
+        <v>37</v>
+      </c>
+      <c r="G2769" s="19">
+        <f t="shared" si="241"/>
+        <v>9</v>
+      </c>
+      <c r="H2769" s="15">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="I2769" s="23">
+        <f t="shared" si="243"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2770" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2770" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2770">
+        <v>55594</v>
+      </c>
+      <c r="D2770">
+        <v>559</v>
+      </c>
+      <c r="E2770">
+        <v>46915</v>
+      </c>
+      <c r="F2770" s="26">
+        <f t="shared" si="240"/>
+        <v>8120</v>
+      </c>
+      <c r="G2770" s="19">
+        <f t="shared" si="241"/>
+        <v>538</v>
+      </c>
+      <c r="H2770" s="15">
+        <f t="shared" si="242"/>
+        <v>2</v>
+      </c>
+      <c r="I2770" s="23">
+        <f t="shared" si="243"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2771" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2771" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2771">
+        <v>84609</v>
+      </c>
+      <c r="D2771">
+        <v>2283</v>
+      </c>
+      <c r="E2771">
+        <v>74470</v>
+      </c>
+      <c r="F2771" s="26">
+        <f t="shared" si="240"/>
+        <v>7856</v>
+      </c>
+      <c r="G2771" s="19">
+        <f t="shared" si="241"/>
+        <v>979</v>
+      </c>
+      <c r="H2771" s="15">
+        <f t="shared" si="242"/>
+        <v>9</v>
+      </c>
+      <c r="I2771" s="23">
+        <f t="shared" si="243"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2772" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2772" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2772">
+        <v>212918</v>
+      </c>
+      <c r="D2772">
+        <v>6229</v>
+      </c>
+      <c r="E2772">
+        <v>184297</v>
+      </c>
+      <c r="F2772" s="26">
+        <f t="shared" si="240"/>
+        <v>22392</v>
+      </c>
+      <c r="G2772" s="19">
+        <f t="shared" si="241"/>
+        <v>2823</v>
+      </c>
+      <c r="H2772" s="15">
+        <f t="shared" si="242"/>
+        <v>39</v>
+      </c>
+      <c r="I2772" s="23">
+        <f t="shared" si="243"/>
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2773" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2773" s="8">
+        <v>44282</v>
+      </c>
+      <c r="C2773">
+        <v>264607</v>
+      </c>
+      <c r="D2773">
+        <v>4491</v>
+      </c>
+      <c r="E2773">
+        <v>255671</v>
+      </c>
+      <c r="F2773" s="26">
+        <f t="shared" si="240"/>
+        <v>4445</v>
+      </c>
+      <c r="G2773" s="19">
+        <f t="shared" si="241"/>
+        <v>252</v>
+      </c>
+      <c r="H2773" s="15">
+        <f t="shared" si="242"/>
+        <v>4</v>
+      </c>
+      <c r="I2773" s="23">
+        <f t="shared" si="243"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2774" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2774" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2774">
+        <v>12484</v>
+      </c>
+      <c r="D2774">
+        <v>348</v>
+      </c>
+      <c r="E2774">
+        <v>10760</v>
+      </c>
+      <c r="F2774" s="26">
+        <f t="shared" si="240"/>
+        <v>1376</v>
+      </c>
+      <c r="G2774" s="19">
+        <f t="shared" si="241"/>
+        <v>117</v>
+      </c>
+      <c r="H2774" s="15">
+        <f t="shared" si="242"/>
+        <v>4</v>
+      </c>
+      <c r="I2774" s="23">
+        <f t="shared" si="243"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2775" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2775" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2775">
+        <v>19525</v>
+      </c>
+      <c r="D2775">
+        <v>206</v>
+      </c>
+      <c r="E2775">
+        <v>19046</v>
+      </c>
+      <c r="F2775" s="26">
+        <f t="shared" ref="F2775:F2794" si="244">C2775-D2775-E2775</f>
+        <v>273</v>
+      </c>
+      <c r="G2775" s="19">
+        <f t="shared" ref="G2775:G2794" si="245">C2775-C2768</f>
+        <v>28</v>
+      </c>
+      <c r="H2775" s="15">
+        <f t="shared" ref="H2775:H2794" si="246">D2775-D2768</f>
+        <v>0</v>
+      </c>
+      <c r="I2775" s="23">
+        <f t="shared" ref="I2775:I2794" si="247">E2775-E2768</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2776" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2776" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2776">
+        <v>5010</v>
+      </c>
+      <c r="D2776">
+        <v>103</v>
+      </c>
+      <c r="E2776">
+        <v>4859</v>
+      </c>
+      <c r="F2776" s="26">
+        <f t="shared" si="244"/>
+        <v>48</v>
+      </c>
+      <c r="G2776" s="19">
+        <f t="shared" si="245"/>
+        <v>11</v>
+      </c>
+      <c r="H2776" s="15">
+        <f t="shared" si="246"/>
+        <v>0</v>
+      </c>
+      <c r="I2776" s="23">
+        <f t="shared" si="247"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2777" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2777" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2777">
+        <v>56450</v>
+      </c>
+      <c r="D2777">
+        <v>561</v>
+      </c>
+      <c r="E2777">
+        <v>47064</v>
+      </c>
+      <c r="F2777" s="26">
+        <f t="shared" si="244"/>
+        <v>8825</v>
+      </c>
+      <c r="G2777" s="19">
+        <f t="shared" si="245"/>
+        <v>856</v>
+      </c>
+      <c r="H2777" s="15">
+        <f t="shared" si="246"/>
+        <v>2</v>
+      </c>
+      <c r="I2777" s="23">
+        <f t="shared" si="247"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2778" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2778" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2778">
+        <v>85531</v>
+      </c>
+      <c r="D2778">
+        <v>2301</v>
+      </c>
+      <c r="E2778">
+        <v>74822</v>
+      </c>
+      <c r="F2778" s="26">
+        <f t="shared" si="244"/>
+        <v>8408</v>
+      </c>
+      <c r="G2778" s="19">
+        <f t="shared" si="245"/>
+        <v>922</v>
+      </c>
+      <c r="H2778" s="15">
+        <f t="shared" si="246"/>
+        <v>18</v>
+      </c>
+      <c r="I2778" s="23">
+        <f t="shared" si="247"/>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2779" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2779" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2779">
+        <v>215227</v>
+      </c>
+      <c r="D2779">
+        <v>6246</v>
+      </c>
+      <c r="E2779">
+        <v>185877</v>
+      </c>
+      <c r="F2779" s="26">
+        <f t="shared" si="244"/>
+        <v>23104</v>
+      </c>
+      <c r="G2779" s="19">
+        <f t="shared" si="245"/>
+        <v>2309</v>
+      </c>
+      <c r="H2779" s="15">
+        <f t="shared" si="246"/>
+        <v>17</v>
+      </c>
+      <c r="I2779" s="23">
+        <f t="shared" si="247"/>
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2780" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2780" s="8">
+        <v>44283</v>
+      </c>
+      <c r="C2780">
+        <v>264889</v>
+      </c>
+      <c r="D2780">
+        <v>4491</v>
+      </c>
+      <c r="E2780">
+        <v>255769</v>
+      </c>
+      <c r="F2780" s="26">
+        <f t="shared" si="244"/>
+        <v>4629</v>
+      </c>
+      <c r="G2780" s="19">
+        <f t="shared" si="245"/>
+        <v>282</v>
+      </c>
+      <c r="H2780" s="15">
+        <f t="shared" si="246"/>
+        <v>0</v>
+      </c>
+      <c r="I2780" s="23">
+        <f t="shared" si="247"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2781" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2781" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2781">
+        <v>12549</v>
+      </c>
+      <c r="D2781">
+        <v>350</v>
+      </c>
+      <c r="E2781">
+        <v>10812</v>
+      </c>
+      <c r="F2781" s="26">
+        <f t="shared" si="244"/>
+        <v>1387</v>
+      </c>
+      <c r="G2781" s="19">
+        <f t="shared" si="245"/>
+        <v>65</v>
+      </c>
+      <c r="H2781" s="15">
+        <f t="shared" si="246"/>
+        <v>2</v>
+      </c>
+      <c r="I2781" s="23">
+        <f t="shared" si="247"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2782" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2782" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2782">
+        <v>19535</v>
+      </c>
+      <c r="D2782">
+        <v>207</v>
+      </c>
+      <c r="E2782">
+        <v>19067</v>
+      </c>
+      <c r="F2782" s="26">
+        <f t="shared" si="244"/>
+        <v>261</v>
+      </c>
+      <c r="G2782" s="19">
+        <f t="shared" si="245"/>
+        <v>10</v>
+      </c>
+      <c r="H2782" s="15">
+        <f t="shared" si="246"/>
+        <v>1</v>
+      </c>
+      <c r="I2782" s="23">
+        <f t="shared" si="247"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2783" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2783" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2783">
+        <v>5016</v>
+      </c>
+      <c r="D2783">
+        <v>103</v>
+      </c>
+      <c r="E2783">
+        <v>4867</v>
+      </c>
+      <c r="F2783" s="26">
+        <f t="shared" si="244"/>
+        <v>46</v>
+      </c>
+      <c r="G2783" s="19">
+        <f t="shared" si="245"/>
+        <v>6</v>
+      </c>
+      <c r="H2783" s="15">
+        <f t="shared" si="246"/>
+        <v>0</v>
+      </c>
+      <c r="I2783" s="23">
+        <f t="shared" si="247"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2784" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2784" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2784">
+        <v>57204</v>
+      </c>
+      <c r="D2784">
+        <v>563</v>
+      </c>
+      <c r="E2784">
+        <v>47271</v>
+      </c>
+      <c r="F2784" s="26">
+        <f t="shared" si="244"/>
+        <v>9370</v>
+      </c>
+      <c r="G2784" s="19">
+        <f t="shared" si="245"/>
+        <v>754</v>
+      </c>
+      <c r="H2784" s="15">
+        <f t="shared" si="246"/>
+        <v>2</v>
+      </c>
+      <c r="I2784" s="23">
+        <f t="shared" si="247"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2785" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2785" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2785">
+        <v>86044</v>
+      </c>
+      <c r="D2785">
+        <v>2319</v>
+      </c>
+      <c r="E2785">
+        <v>75324</v>
+      </c>
+      <c r="F2785" s="26">
+        <f t="shared" si="244"/>
+        <v>8401</v>
+      </c>
+      <c r="G2785" s="19">
+        <f t="shared" si="245"/>
+        <v>513</v>
+      </c>
+      <c r="H2785" s="15">
+        <f t="shared" si="246"/>
+        <v>18</v>
+      </c>
+      <c r="I2785" s="23">
+        <f t="shared" si="247"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2786" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2786" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2786">
+        <v>217694</v>
+      </c>
+      <c r="D2786">
+        <v>6319</v>
+      </c>
+      <c r="E2786">
+        <v>186985</v>
+      </c>
+      <c r="F2786" s="26">
+        <f t="shared" si="244"/>
+        <v>24390</v>
+      </c>
+      <c r="G2786" s="19">
+        <f t="shared" si="245"/>
+        <v>2467</v>
+      </c>
+      <c r="H2786" s="15">
+        <f t="shared" si="246"/>
+        <v>73</v>
+      </c>
+      <c r="I2786" s="23">
+        <f t="shared" si="247"/>
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2787" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2787" s="8">
+        <v>44284</v>
+      </c>
+      <c r="C2787">
+        <v>265158</v>
+      </c>
+      <c r="D2787">
+        <v>4495</v>
+      </c>
+      <c r="E2787">
+        <v>255952</v>
+      </c>
+      <c r="F2787" s="26">
+        <f t="shared" si="244"/>
+        <v>4711</v>
+      </c>
+      <c r="G2787" s="19">
+        <f t="shared" si="245"/>
+        <v>269</v>
+      </c>
+      <c r="H2787" s="15">
+        <f t="shared" si="246"/>
+        <v>4</v>
+      </c>
+      <c r="I2787" s="23">
+        <f t="shared" si="247"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2788" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2788" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2788">
+        <v>12663</v>
+      </c>
+      <c r="D2788">
+        <v>352</v>
+      </c>
+      <c r="E2788">
+        <v>10865</v>
+      </c>
+      <c r="F2788" s="26">
+        <f t="shared" si="244"/>
+        <v>1446</v>
+      </c>
+      <c r="G2788" s="19">
+        <f t="shared" si="245"/>
+        <v>114</v>
+      </c>
+      <c r="H2788" s="15">
+        <f t="shared" si="246"/>
+        <v>2</v>
+      </c>
+      <c r="I2788" s="23">
+        <f t="shared" si="247"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2789" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2789" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2789">
+        <v>19557</v>
+      </c>
+      <c r="D2789">
+        <v>207</v>
+      </c>
+      <c r="E2789">
+        <v>19090</v>
+      </c>
+      <c r="F2789" s="26">
+        <f t="shared" si="244"/>
+        <v>260</v>
+      </c>
+      <c r="G2789" s="19">
+        <f t="shared" si="245"/>
+        <v>22</v>
+      </c>
+      <c r="H2789" s="15">
+        <f t="shared" si="246"/>
+        <v>0</v>
+      </c>
+      <c r="I2789" s="23">
+        <f t="shared" si="247"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2790" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2790" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2790">
+        <v>5024</v>
+      </c>
+      <c r="D2790">
+        <v>103</v>
+      </c>
+      <c r="E2790">
+        <v>4867</v>
+      </c>
+      <c r="F2790" s="26">
+        <f t="shared" si="244"/>
+        <v>54</v>
+      </c>
+      <c r="G2790" s="19">
+        <f t="shared" si="245"/>
+        <v>8</v>
+      </c>
+      <c r="H2790" s="15">
+        <f t="shared" si="246"/>
+        <v>0</v>
+      </c>
+      <c r="I2790" s="23">
+        <f t="shared" si="247"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2791" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2791" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2791">
+        <v>57833</v>
+      </c>
+      <c r="D2791">
+        <v>568</v>
+      </c>
+      <c r="E2791">
+        <v>47458</v>
+      </c>
+      <c r="F2791" s="26">
+        <f t="shared" si="244"/>
+        <v>9807</v>
+      </c>
+      <c r="G2791" s="19">
+        <f t="shared" si="245"/>
+        <v>629</v>
+      </c>
+      <c r="H2791" s="15">
+        <f t="shared" si="246"/>
+        <v>5</v>
+      </c>
+      <c r="I2791" s="23">
+        <f t="shared" si="247"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2792" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2792" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2792">
+        <v>87055</v>
+      </c>
+      <c r="D2792">
+        <v>2342</v>
+      </c>
+      <c r="E2792">
+        <v>76232</v>
+      </c>
+      <c r="F2792" s="26">
+        <f t="shared" si="244"/>
+        <v>8481</v>
+      </c>
+      <c r="G2792" s="19">
+        <f t="shared" si="245"/>
+        <v>1011</v>
+      </c>
+      <c r="H2792" s="15">
+        <f t="shared" si="246"/>
+        <v>23</v>
+      </c>
+      <c r="I2792" s="23">
+        <f t="shared" si="247"/>
+        <v>908</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2793" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2793" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2793">
+        <v>220392</v>
+      </c>
+      <c r="D2793">
+        <v>6365</v>
+      </c>
+      <c r="E2793">
+        <v>188562</v>
+      </c>
+      <c r="F2793" s="26">
+        <f t="shared" si="244"/>
+        <v>25465</v>
+      </c>
+      <c r="G2793" s="19">
+        <f t="shared" si="245"/>
+        <v>2698</v>
+      </c>
+      <c r="H2793" s="15">
+        <f t="shared" si="246"/>
+        <v>46</v>
+      </c>
+      <c r="I2793" s="23">
+        <f t="shared" si="247"/>
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2794" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2794" s="8">
+        <v>44285</v>
+      </c>
+      <c r="C2794">
+        <v>265433</v>
+      </c>
+      <c r="D2794">
+        <v>4497</v>
+      </c>
+      <c r="E2794">
+        <v>256052</v>
+      </c>
+      <c r="F2794" s="26">
+        <f t="shared" si="244"/>
+        <v>4884</v>
+      </c>
+      <c r="G2794" s="19">
+        <f t="shared" si="245"/>
+        <v>275</v>
+      </c>
+      <c r="H2794" s="15">
+        <f t="shared" si="246"/>
+        <v>2</v>
+      </c>
+      <c r="I2794" s="23">
+        <f t="shared" si="247"/>
+        <v>100</v>
+      </c>
+    </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1048576" s="8">
         <v>44269</v>

</xml_diff>